<commit_message>
update xls load factor to 4
</commit_message>
<xml_diff>
--- a/resources/tools/YARNCalcs.xlsx
+++ b/resources/tools/YARNCalcs.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -609,7 +611,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
@@ -631,7 +633,7 @@
       </c>
       <c r="F2" s="7">
         <f>MIN(C15,PRODUCT(B2,2))</f>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1">
@@ -639,7 +641,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="2">
-        <v>256</v>
+        <v>128</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="6" t="s">
@@ -647,7 +649,7 @@
       </c>
       <c r="F3" s="7">
         <f>PRODUCT(B15,1024)</f>
-        <v>232857.60000000001</v>
+        <v>98508.800000000003</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
@@ -669,7 +671,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="6" t="s">
@@ -710,7 +712,7 @@
       </c>
       <c r="B8" s="7">
         <f>PRODUCT(0.1,B3)</f>
-        <v>25.6</v>
+        <v>12.8</v>
       </c>
       <c r="C8" s="6">
         <v>2</v>
@@ -739,7 +741,7 @@
       </c>
       <c r="F9" s="11">
         <f>PRODUCT(F2,1024)</f>
-        <v>24576</v>
+        <v>22528</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
@@ -765,10 +767,10 @@
         <v>20</v>
       </c>
       <c r="B11" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C11" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="8" t="s">
@@ -798,7 +800,7 @@
       </c>
       <c r="G12" s="7">
         <f>F3/F12</f>
-        <v>227.4</v>
+        <v>96.2</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1">
@@ -841,7 +843,7 @@
       </c>
       <c r="G14" s="7">
         <f>F2/F14</f>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1">
@@ -850,11 +852,11 @@
       </c>
       <c r="B15" s="7">
         <f>SUM(B3,-B8,-B9,-B10,-B11,-B12,-B13,-B14)</f>
-        <v>227.4</v>
+        <v>96.2</v>
       </c>
       <c r="C15" s="7">
         <f>SUM(B1,-C8,-C9,-C10,-C11,-C12,-C13,-C14)</f>
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="13" t="s">
@@ -970,7 +972,7 @@
       </c>
       <c r="F27" s="11">
         <f>MIN(G12,G14,PRODUCT(B4,B5))</f>
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="4:7" ht="15.75" customHeight="1">
@@ -980,7 +982,7 @@
       </c>
       <c r="F28" s="11">
         <f>MIN(G12,G14,PRODUCT(B4,B5))</f>
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="4:7" ht="15.75" customHeight="1">

</xml_diff>